<commit_message>
fix view area home
</commit_message>
<xml_diff>
--- a/resources/report-booking.xlsx
+++ b/resources/report-booking.xlsx
@@ -15,9 +15,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
-  <si>
-    <t>LỊCH ĐẶT PHÒNG TỪ NGÀY (11/07/2016 - 17/07/2016)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="56">
+  <si>
+    <t>LỊCH ĐẶT PHÒNG TỪ NGÀY (20/07/2015 - 20/07/2016)</t>
   </si>
   <si>
     <t>STT</t>
@@ -29,31 +29,157 @@
     <t>Phòng</t>
   </si>
   <si>
-    <t>11/07</t>
-  </si>
-  <si>
-    <t>12/07</t>
-  </si>
-  <si>
-    <t>13/07</t>
-  </si>
-  <si>
-    <t>14/07</t>
-  </si>
-  <si>
-    <t>15/07</t>
-  </si>
-  <si>
-    <t>16/07</t>
-  </si>
-  <si>
-    <t>17/07</t>
-  </si>
-  <si>
-    <t>Villa Santai - Kuta - 4 Bedrooms</t>
+    <t>20/07</t>
+  </si>
+  <si>
+    <t>21/07</t>
+  </si>
+  <si>
+    <t>22/07</t>
+  </si>
+  <si>
+    <t>23/07</t>
+  </si>
+  <si>
+    <t>24/07</t>
+  </si>
+  <si>
+    <t>25/07</t>
+  </si>
+  <si>
+    <t>26/07</t>
+  </si>
+  <si>
+    <t>27/07</t>
+  </si>
+  <si>
+    <t>28/07</t>
+  </si>
+  <si>
+    <t>29/07</t>
+  </si>
+  <si>
+    <t>30/07</t>
+  </si>
+  <si>
+    <t>31/07</t>
+  </si>
+  <si>
+    <t>01/08</t>
+  </si>
+  <si>
+    <t>02/08</t>
+  </si>
+  <si>
+    <t>03/08</t>
+  </si>
+  <si>
+    <t>04/08</t>
+  </si>
+  <si>
+    <t>05/08</t>
+  </si>
+  <si>
+    <t>06/08</t>
+  </si>
+  <si>
+    <t>07/08</t>
+  </si>
+  <si>
+    <t>08/08</t>
+  </si>
+  <si>
+    <t>09/08</t>
+  </si>
+  <si>
+    <t>10/08</t>
+  </si>
+  <si>
+    <t>11/08</t>
+  </si>
+  <si>
+    <t>12/08</t>
+  </si>
+  <si>
+    <t>13/08</t>
+  </si>
+  <si>
+    <t>14/08</t>
+  </si>
+  <si>
+    <t>15/08</t>
+  </si>
+  <si>
+    <t>16/08</t>
+  </si>
+  <si>
+    <t>17/08</t>
+  </si>
+  <si>
+    <t>18/08</t>
+  </si>
+  <si>
+    <t>19/08</t>
+  </si>
+  <si>
+    <t>20/08</t>
+  </si>
+  <si>
+    <t>21/08</t>
+  </si>
+  <si>
+    <t>22/08</t>
+  </si>
+  <si>
+    <t>23/08</t>
+  </si>
+  <si>
+    <t>24/08</t>
+  </si>
+  <si>
+    <t>25/08</t>
+  </si>
+  <si>
+    <t>26/08</t>
+  </si>
+  <si>
+    <t>27/08</t>
+  </si>
+  <si>
+    <t>28/08</t>
+  </si>
+  <si>
+    <t>29/08</t>
+  </si>
+  <si>
+    <t>30/08</t>
+  </si>
+  <si>
+    <t>31/08</t>
+  </si>
+  <si>
+    <t>01/09</t>
+  </si>
+  <si>
+    <t>02/09</t>
+  </si>
+  <si>
+    <t>03/09</t>
+  </si>
+  <si>
+    <t>04/09</t>
+  </si>
+  <si>
+    <t>05/09</t>
+  </si>
+  <si>
+    <t>Villa Santai Kuta 4 Bedrooms</t>
   </si>
   <si>
     <t>Nguyên căn</t>
+  </si>
+  <si>
+    <t>Delightful &amp; Cozy Villa Umalas</t>
   </si>
   <si>
     <t>Tổng số khách theo ngày</t>
@@ -398,7 +524,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:AZ5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -407,11 +533,11 @@
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="4.570313" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="38.847656" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="36.419678" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="12.854004" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:52">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -441,7 +567,7 @@
       <c r="Y1"/>
       <c r="Z1"/>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:52">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -472,28 +598,154 @@
       <c r="J2" t="s">
         <v>10</v>
       </c>
+      <c r="K2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>17</v>
+      </c>
+      <c r="R2" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" t="s">
+        <v>19</v>
+      </c>
+      <c r="T2" t="s">
+        <v>20</v>
+      </c>
+      <c r="U2" t="s">
+        <v>21</v>
+      </c>
+      <c r="V2" t="s">
+        <v>22</v>
+      </c>
+      <c r="W2" t="s">
+        <v>23</v>
+      </c>
+      <c r="X2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:52">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="D3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -504,24 +756,154 @@
       <c r="J3">
         <v>0</v>
       </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
+        <v>0</v>
+      </c>
+      <c r="AG3">
+        <v>0</v>
+      </c>
+      <c r="AH3">
+        <v>0</v>
+      </c>
+      <c r="AI3">
+        <v>0</v>
+      </c>
+      <c r="AJ3">
+        <v>0</v>
+      </c>
+      <c r="AK3">
+        <v>0</v>
+      </c>
+      <c r="AL3">
+        <v>0</v>
+      </c>
+      <c r="AM3">
+        <v>0</v>
+      </c>
+      <c r="AN3">
+        <v>0</v>
+      </c>
+      <c r="AO3">
+        <v>0</v>
+      </c>
+      <c r="AP3">
+        <v>0</v>
+      </c>
+      <c r="AQ3">
+        <v>0</v>
+      </c>
+      <c r="AR3">
+        <v>0</v>
+      </c>
+      <c r="AS3">
+        <v>0</v>
+      </c>
+      <c r="AT3">
+        <v>0</v>
+      </c>
+      <c r="AU3">
+        <v>0</v>
+      </c>
+      <c r="AV3">
+        <v>0</v>
+      </c>
+      <c r="AW3">
+        <v>0</v>
+      </c>
+      <c r="AX3">
+        <v>0</v>
+      </c>
+      <c r="AY3">
+        <v>0</v>
+      </c>
+      <c r="AZ3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:26">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4"/>
-      <c r="C4"/>
+    <row r="4" spans="1:52">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>53</v>
+      </c>
       <c r="D4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -530,6 +912,286 @@
         <v>0</v>
       </c>
       <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <v>0</v>
+      </c>
+      <c r="AF4">
+        <v>0</v>
+      </c>
+      <c r="AG4">
+        <v>0</v>
+      </c>
+      <c r="AH4">
+        <v>0</v>
+      </c>
+      <c r="AI4">
+        <v>0</v>
+      </c>
+      <c r="AJ4">
+        <v>0</v>
+      </c>
+      <c r="AK4">
+        <v>0</v>
+      </c>
+      <c r="AL4">
+        <v>0</v>
+      </c>
+      <c r="AM4">
+        <v>0</v>
+      </c>
+      <c r="AN4">
+        <v>0</v>
+      </c>
+      <c r="AO4">
+        <v>0</v>
+      </c>
+      <c r="AP4">
+        <v>0</v>
+      </c>
+      <c r="AQ4">
+        <v>0</v>
+      </c>
+      <c r="AR4">
+        <v>0</v>
+      </c>
+      <c r="AS4">
+        <v>0</v>
+      </c>
+      <c r="AT4">
+        <v>0</v>
+      </c>
+      <c r="AU4">
+        <v>0</v>
+      </c>
+      <c r="AV4">
+        <v>0</v>
+      </c>
+      <c r="AW4">
+        <v>0</v>
+      </c>
+      <c r="AX4">
+        <v>0</v>
+      </c>
+      <c r="AY4">
+        <v>0</v>
+      </c>
+      <c r="AZ4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:52">
+      <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5"/>
+      <c r="C5"/>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+      <c r="AE5">
+        <v>0</v>
+      </c>
+      <c r="AF5">
+        <v>0</v>
+      </c>
+      <c r="AG5">
+        <v>0</v>
+      </c>
+      <c r="AH5">
+        <v>0</v>
+      </c>
+      <c r="AI5">
+        <v>0</v>
+      </c>
+      <c r="AJ5">
+        <v>0</v>
+      </c>
+      <c r="AK5">
+        <v>0</v>
+      </c>
+      <c r="AL5">
+        <v>0</v>
+      </c>
+      <c r="AM5">
+        <v>0</v>
+      </c>
+      <c r="AN5">
+        <v>0</v>
+      </c>
+      <c r="AO5">
+        <v>0</v>
+      </c>
+      <c r="AP5">
+        <v>0</v>
+      </c>
+      <c r="AQ5">
+        <v>0</v>
+      </c>
+      <c r="AR5">
+        <v>0</v>
+      </c>
+      <c r="AS5">
+        <v>0</v>
+      </c>
+      <c r="AT5">
+        <v>0</v>
+      </c>
+      <c r="AU5">
+        <v>0</v>
+      </c>
+      <c r="AV5">
+        <v>0</v>
+      </c>
+      <c r="AW5">
+        <v>0</v>
+      </c>
+      <c r="AX5">
+        <v>0</v>
+      </c>
+      <c r="AY5">
+        <v>0</v>
+      </c>
+      <c r="AZ5">
         <v>0</v>
       </c>
     </row>
@@ -537,7 +1199,7 @@
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <mergeCells>
     <mergeCell ref="A1:Z1"/>
-    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>